<commit_message>
Updating spreadsheet with more data
</commit_message>
<xml_diff>
--- a/Universe_revenues_EXAMPLE_OUTPUT.xlsx
+++ b/Universe_revenues_EXAMPLE_OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="672">
   <si>
     <t>Ticker</t>
   </si>
@@ -2027,6 +2027,9 @@
   </si>
   <si>
     <t>N/D</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -7623,20 +7626,20 @@
       <c r="C202" t="s">
         <v>538</v>
       </c>
-      <c r="D202">
-        <v>0</v>
-      </c>
-      <c r="E202">
-        <v>0</v>
-      </c>
-      <c r="F202">
-        <v>0</v>
-      </c>
-      <c r="G202">
-        <v>0</v>
-      </c>
-      <c r="H202">
-        <v>0</v>
+      <c r="D202" t="s">
+        <v>671</v>
+      </c>
+      <c r="E202" t="s">
+        <v>671</v>
+      </c>
+      <c r="F202" t="s">
+        <v>671</v>
+      </c>
+      <c r="G202" t="s">
+        <v>671</v>
+      </c>
+      <c r="H202" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7649,20 +7652,20 @@
       <c r="C203" t="s">
         <v>539</v>
       </c>
-      <c r="D203">
-        <v>0</v>
-      </c>
-      <c r="E203">
-        <v>0</v>
-      </c>
-      <c r="F203">
-        <v>0</v>
-      </c>
-      <c r="G203">
-        <v>0</v>
-      </c>
-      <c r="H203">
-        <v>0</v>
+      <c r="D203" t="s">
+        <v>671</v>
+      </c>
+      <c r="E203" t="s">
+        <v>671</v>
+      </c>
+      <c r="F203" t="s">
+        <v>671</v>
+      </c>
+      <c r="G203" t="s">
+        <v>671</v>
+      </c>
+      <c r="H203" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7675,20 +7678,20 @@
       <c r="C204" t="s">
         <v>540</v>
       </c>
-      <c r="D204">
-        <v>0</v>
-      </c>
-      <c r="E204">
-        <v>0</v>
-      </c>
-      <c r="F204">
-        <v>0</v>
-      </c>
-      <c r="G204">
-        <v>0</v>
-      </c>
-      <c r="H204">
-        <v>0</v>
+      <c r="D204" t="s">
+        <v>671</v>
+      </c>
+      <c r="E204" t="s">
+        <v>671</v>
+      </c>
+      <c r="F204" t="s">
+        <v>671</v>
+      </c>
+      <c r="G204" t="s">
+        <v>671</v>
+      </c>
+      <c r="H204" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7701,20 +7704,20 @@
       <c r="C205" t="s">
         <v>541</v>
       </c>
-      <c r="D205">
-        <v>0</v>
-      </c>
-      <c r="E205">
-        <v>0</v>
-      </c>
-      <c r="F205">
-        <v>0</v>
-      </c>
-      <c r="G205">
-        <v>0</v>
-      </c>
-      <c r="H205">
-        <v>0</v>
+      <c r="D205" t="s">
+        <v>671</v>
+      </c>
+      <c r="E205" t="s">
+        <v>671</v>
+      </c>
+      <c r="F205" t="s">
+        <v>671</v>
+      </c>
+      <c r="G205" t="s">
+        <v>671</v>
+      </c>
+      <c r="H205" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7727,20 +7730,20 @@
       <c r="C206" t="s">
         <v>542</v>
       </c>
-      <c r="D206">
-        <v>0</v>
-      </c>
-      <c r="E206">
-        <v>0</v>
-      </c>
-      <c r="F206">
-        <v>0</v>
-      </c>
-      <c r="G206">
-        <v>0</v>
-      </c>
-      <c r="H206">
-        <v>0</v>
+      <c r="D206" t="s">
+        <v>671</v>
+      </c>
+      <c r="E206" t="s">
+        <v>671</v>
+      </c>
+      <c r="F206" t="s">
+        <v>671</v>
+      </c>
+      <c r="G206" t="s">
+        <v>671</v>
+      </c>
+      <c r="H206" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7753,20 +7756,20 @@
       <c r="C207" t="s">
         <v>502</v>
       </c>
-      <c r="D207">
-        <v>0</v>
-      </c>
-      <c r="E207">
-        <v>0</v>
-      </c>
-      <c r="F207">
-        <v>0</v>
-      </c>
-      <c r="G207">
-        <v>0</v>
-      </c>
-      <c r="H207">
-        <v>0</v>
+      <c r="D207" t="s">
+        <v>671</v>
+      </c>
+      <c r="E207" t="s">
+        <v>671</v>
+      </c>
+      <c r="F207" t="s">
+        <v>671</v>
+      </c>
+      <c r="G207" t="s">
+        <v>671</v>
+      </c>
+      <c r="H207" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7779,20 +7782,20 @@
       <c r="C208" t="s">
         <v>543</v>
       </c>
-      <c r="D208">
-        <v>0</v>
-      </c>
-      <c r="E208">
-        <v>0</v>
-      </c>
-      <c r="F208">
-        <v>0</v>
-      </c>
-      <c r="G208">
-        <v>0</v>
-      </c>
-      <c r="H208">
-        <v>0</v>
+      <c r="D208" t="s">
+        <v>671</v>
+      </c>
+      <c r="E208" t="s">
+        <v>671</v>
+      </c>
+      <c r="F208" t="s">
+        <v>671</v>
+      </c>
+      <c r="G208" t="s">
+        <v>671</v>
+      </c>
+      <c r="H208" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7805,20 +7808,20 @@
       <c r="C209" t="s">
         <v>544</v>
       </c>
-      <c r="D209">
-        <v>0</v>
-      </c>
-      <c r="E209">
-        <v>0</v>
-      </c>
-      <c r="F209">
-        <v>0</v>
-      </c>
-      <c r="G209">
-        <v>0</v>
-      </c>
-      <c r="H209">
-        <v>0</v>
+      <c r="D209" t="s">
+        <v>671</v>
+      </c>
+      <c r="E209" t="s">
+        <v>671</v>
+      </c>
+      <c r="F209" t="s">
+        <v>671</v>
+      </c>
+      <c r="G209" t="s">
+        <v>671</v>
+      </c>
+      <c r="H209" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7831,20 +7834,20 @@
       <c r="C210" t="s">
         <v>545</v>
       </c>
-      <c r="D210">
-        <v>0</v>
-      </c>
-      <c r="E210">
-        <v>0</v>
-      </c>
-      <c r="F210">
-        <v>0</v>
-      </c>
-      <c r="G210">
-        <v>0</v>
-      </c>
-      <c r="H210">
-        <v>0</v>
+      <c r="D210" t="s">
+        <v>671</v>
+      </c>
+      <c r="E210" t="s">
+        <v>671</v>
+      </c>
+      <c r="F210" t="s">
+        <v>671</v>
+      </c>
+      <c r="G210" t="s">
+        <v>671</v>
+      </c>
+      <c r="H210" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7857,20 +7860,20 @@
       <c r="C211" t="s">
         <v>546</v>
       </c>
-      <c r="D211">
-        <v>0</v>
-      </c>
-      <c r="E211">
-        <v>0</v>
-      </c>
-      <c r="F211">
-        <v>0</v>
-      </c>
-      <c r="G211">
-        <v>0</v>
-      </c>
-      <c r="H211">
-        <v>0</v>
+      <c r="D211" t="s">
+        <v>671</v>
+      </c>
+      <c r="E211" t="s">
+        <v>671</v>
+      </c>
+      <c r="F211" t="s">
+        <v>671</v>
+      </c>
+      <c r="G211" t="s">
+        <v>671</v>
+      </c>
+      <c r="H211" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7883,20 +7886,20 @@
       <c r="C212" t="s">
         <v>546</v>
       </c>
-      <c r="D212">
-        <v>0</v>
-      </c>
-      <c r="E212">
-        <v>0</v>
-      </c>
-      <c r="F212">
-        <v>0</v>
-      </c>
-      <c r="G212">
-        <v>0</v>
-      </c>
-      <c r="H212">
-        <v>0</v>
+      <c r="D212" t="s">
+        <v>671</v>
+      </c>
+      <c r="E212" t="s">
+        <v>671</v>
+      </c>
+      <c r="F212" t="s">
+        <v>671</v>
+      </c>
+      <c r="G212" t="s">
+        <v>671</v>
+      </c>
+      <c r="H212" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7909,20 +7912,20 @@
       <c r="C213" t="s">
         <v>547</v>
       </c>
-      <c r="D213">
-        <v>0</v>
-      </c>
-      <c r="E213">
-        <v>0</v>
-      </c>
-      <c r="F213">
-        <v>0</v>
-      </c>
-      <c r="G213">
-        <v>0</v>
-      </c>
-      <c r="H213">
-        <v>0</v>
+      <c r="D213" t="s">
+        <v>671</v>
+      </c>
+      <c r="E213" t="s">
+        <v>671</v>
+      </c>
+      <c r="F213" t="s">
+        <v>671</v>
+      </c>
+      <c r="G213" t="s">
+        <v>671</v>
+      </c>
+      <c r="H213" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7935,20 +7938,20 @@
       <c r="C214" t="s">
         <v>548</v>
       </c>
-      <c r="D214">
-        <v>0</v>
-      </c>
-      <c r="E214">
-        <v>0</v>
-      </c>
-      <c r="F214">
-        <v>0</v>
-      </c>
-      <c r="G214">
-        <v>0</v>
-      </c>
-      <c r="H214">
-        <v>0</v>
+      <c r="D214" t="s">
+        <v>671</v>
+      </c>
+      <c r="E214" t="s">
+        <v>671</v>
+      </c>
+      <c r="F214" t="s">
+        <v>671</v>
+      </c>
+      <c r="G214" t="s">
+        <v>671</v>
+      </c>
+      <c r="H214" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7961,20 +7964,20 @@
       <c r="C215" t="s">
         <v>549</v>
       </c>
-      <c r="D215">
-        <v>0</v>
-      </c>
-      <c r="E215">
-        <v>0</v>
-      </c>
-      <c r="F215">
-        <v>0</v>
-      </c>
-      <c r="G215">
-        <v>0</v>
-      </c>
-      <c r="H215">
-        <v>0</v>
+      <c r="D215" t="s">
+        <v>671</v>
+      </c>
+      <c r="E215" t="s">
+        <v>671</v>
+      </c>
+      <c r="F215" t="s">
+        <v>671</v>
+      </c>
+      <c r="G215" t="s">
+        <v>671</v>
+      </c>
+      <c r="H215" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7987,20 +7990,20 @@
       <c r="C216" t="s">
         <v>550</v>
       </c>
-      <c r="D216">
-        <v>0</v>
-      </c>
-      <c r="E216">
-        <v>0</v>
-      </c>
-      <c r="F216">
-        <v>0</v>
-      </c>
-      <c r="G216">
-        <v>0</v>
-      </c>
-      <c r="H216">
-        <v>0</v>
+      <c r="D216" t="s">
+        <v>671</v>
+      </c>
+      <c r="E216" t="s">
+        <v>671</v>
+      </c>
+      <c r="F216" t="s">
+        <v>671</v>
+      </c>
+      <c r="G216" t="s">
+        <v>671</v>
+      </c>
+      <c r="H216" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -8013,20 +8016,20 @@
       <c r="C217" t="s">
         <v>551</v>
       </c>
-      <c r="D217">
-        <v>0</v>
-      </c>
-      <c r="E217">
-        <v>0</v>
-      </c>
-      <c r="F217">
-        <v>0</v>
-      </c>
-      <c r="G217">
-        <v>0</v>
-      </c>
-      <c r="H217">
-        <v>0</v>
+      <c r="D217" t="s">
+        <v>671</v>
+      </c>
+      <c r="E217" t="s">
+        <v>671</v>
+      </c>
+      <c r="F217" t="s">
+        <v>671</v>
+      </c>
+      <c r="G217" t="s">
+        <v>671</v>
+      </c>
+      <c r="H217" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -8039,20 +8042,20 @@
       <c r="C218" t="s">
         <v>552</v>
       </c>
-      <c r="D218">
-        <v>0</v>
-      </c>
-      <c r="E218">
-        <v>0</v>
-      </c>
-      <c r="F218">
-        <v>0</v>
-      </c>
-      <c r="G218">
-        <v>0</v>
-      </c>
-      <c r="H218">
-        <v>0</v>
+      <c r="D218" t="s">
+        <v>671</v>
+      </c>
+      <c r="E218" t="s">
+        <v>671</v>
+      </c>
+      <c r="F218" t="s">
+        <v>671</v>
+      </c>
+      <c r="G218" t="s">
+        <v>671</v>
+      </c>
+      <c r="H218" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -8065,20 +8068,20 @@
       <c r="C219" t="s">
         <v>553</v>
       </c>
-      <c r="D219">
-        <v>0</v>
-      </c>
-      <c r="E219">
-        <v>0</v>
-      </c>
-      <c r="F219">
-        <v>0</v>
-      </c>
-      <c r="G219">
-        <v>0</v>
-      </c>
-      <c r="H219">
-        <v>0</v>
+      <c r="D219" t="s">
+        <v>671</v>
+      </c>
+      <c r="E219" t="s">
+        <v>671</v>
+      </c>
+      <c r="F219" t="s">
+        <v>671</v>
+      </c>
+      <c r="G219" t="s">
+        <v>671</v>
+      </c>
+      <c r="H219" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -8091,20 +8094,20 @@
       <c r="C220" t="s">
         <v>554</v>
       </c>
-      <c r="D220">
-        <v>0</v>
-      </c>
-      <c r="E220">
-        <v>0</v>
-      </c>
-      <c r="F220">
-        <v>0</v>
-      </c>
-      <c r="G220">
-        <v>0</v>
-      </c>
-      <c r="H220">
-        <v>0</v>
+      <c r="D220" t="s">
+        <v>671</v>
+      </c>
+      <c r="E220" t="s">
+        <v>671</v>
+      </c>
+      <c r="F220" t="s">
+        <v>671</v>
+      </c>
+      <c r="G220" t="s">
+        <v>671</v>
+      </c>
+      <c r="H220" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -8117,20 +8120,20 @@
       <c r="C221" t="s">
         <v>555</v>
       </c>
-      <c r="D221">
-        <v>0</v>
-      </c>
-      <c r="E221">
-        <v>0</v>
-      </c>
-      <c r="F221">
-        <v>0</v>
-      </c>
-      <c r="G221">
-        <v>0</v>
-      </c>
-      <c r="H221">
-        <v>0</v>
+      <c r="D221" t="s">
+        <v>671</v>
+      </c>
+      <c r="E221" t="s">
+        <v>671</v>
+      </c>
+      <c r="F221" t="s">
+        <v>671</v>
+      </c>
+      <c r="G221" t="s">
+        <v>671</v>
+      </c>
+      <c r="H221" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -8143,20 +8146,20 @@
       <c r="C222" t="s">
         <v>556</v>
       </c>
-      <c r="D222">
-        <v>0</v>
-      </c>
-      <c r="E222">
-        <v>0</v>
-      </c>
-      <c r="F222">
-        <v>0</v>
-      </c>
-      <c r="G222">
-        <v>0</v>
-      </c>
-      <c r="H222">
-        <v>0</v>
+      <c r="D222" t="s">
+        <v>671</v>
+      </c>
+      <c r="E222" t="s">
+        <v>671</v>
+      </c>
+      <c r="F222" t="s">
+        <v>671</v>
+      </c>
+      <c r="G222" t="s">
+        <v>671</v>
+      </c>
+      <c r="H222" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -8169,20 +8172,20 @@
       <c r="C223" t="s">
         <v>557</v>
       </c>
-      <c r="D223">
-        <v>0</v>
-      </c>
-      <c r="E223">
-        <v>0</v>
-      </c>
-      <c r="F223">
-        <v>0</v>
-      </c>
-      <c r="G223">
-        <v>0</v>
-      </c>
-      <c r="H223">
-        <v>0</v>
+      <c r="D223" t="s">
+        <v>671</v>
+      </c>
+      <c r="E223" t="s">
+        <v>671</v>
+      </c>
+      <c r="F223" t="s">
+        <v>671</v>
+      </c>
+      <c r="G223" t="s">
+        <v>671</v>
+      </c>
+      <c r="H223" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -8195,20 +8198,20 @@
       <c r="C224" t="s">
         <v>558</v>
       </c>
-      <c r="D224">
-        <v>0</v>
-      </c>
-      <c r="E224">
-        <v>0</v>
-      </c>
-      <c r="F224">
-        <v>0</v>
-      </c>
-      <c r="G224">
-        <v>0</v>
-      </c>
-      <c r="H224">
-        <v>0</v>
+      <c r="D224" t="s">
+        <v>671</v>
+      </c>
+      <c r="E224" t="s">
+        <v>671</v>
+      </c>
+      <c r="F224" t="s">
+        <v>671</v>
+      </c>
+      <c r="G224" t="s">
+        <v>671</v>
+      </c>
+      <c r="H224" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -8221,20 +8224,20 @@
       <c r="C225" t="s">
         <v>559</v>
       </c>
-      <c r="D225">
-        <v>0</v>
-      </c>
-      <c r="E225">
-        <v>0</v>
-      </c>
-      <c r="F225">
-        <v>0</v>
-      </c>
-      <c r="G225">
-        <v>0</v>
-      </c>
-      <c r="H225">
-        <v>0</v>
+      <c r="D225" t="s">
+        <v>671</v>
+      </c>
+      <c r="E225" t="s">
+        <v>671</v>
+      </c>
+      <c r="F225" t="s">
+        <v>671</v>
+      </c>
+      <c r="G225" t="s">
+        <v>671</v>
+      </c>
+      <c r="H225" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -8247,20 +8250,20 @@
       <c r="C226" t="s">
         <v>560</v>
       </c>
-      <c r="D226">
-        <v>0</v>
-      </c>
-      <c r="E226">
-        <v>0</v>
-      </c>
-      <c r="F226">
-        <v>0</v>
-      </c>
-      <c r="G226">
-        <v>0</v>
-      </c>
-      <c r="H226">
-        <v>0</v>
+      <c r="D226" t="s">
+        <v>671</v>
+      </c>
+      <c r="E226" t="s">
+        <v>671</v>
+      </c>
+      <c r="F226" t="s">
+        <v>671</v>
+      </c>
+      <c r="G226" t="s">
+        <v>671</v>
+      </c>
+      <c r="H226" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -8273,20 +8276,20 @@
       <c r="C227" t="s">
         <v>561</v>
       </c>
-      <c r="D227">
-        <v>0</v>
-      </c>
-      <c r="E227">
-        <v>0</v>
-      </c>
-      <c r="F227">
-        <v>0</v>
-      </c>
-      <c r="G227">
-        <v>0</v>
-      </c>
-      <c r="H227">
-        <v>0</v>
+      <c r="D227" t="s">
+        <v>671</v>
+      </c>
+      <c r="E227" t="s">
+        <v>671</v>
+      </c>
+      <c r="F227" t="s">
+        <v>671</v>
+      </c>
+      <c r="G227" t="s">
+        <v>671</v>
+      </c>
+      <c r="H227" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -8299,20 +8302,20 @@
       <c r="C228" t="s">
         <v>562</v>
       </c>
-      <c r="D228">
-        <v>0</v>
-      </c>
-      <c r="E228">
-        <v>0</v>
-      </c>
-      <c r="F228">
-        <v>0</v>
-      </c>
-      <c r="G228">
-        <v>0</v>
-      </c>
-      <c r="H228">
-        <v>0</v>
+      <c r="D228" t="s">
+        <v>671</v>
+      </c>
+      <c r="E228" t="s">
+        <v>671</v>
+      </c>
+      <c r="F228" t="s">
+        <v>671</v>
+      </c>
+      <c r="G228" t="s">
+        <v>671</v>
+      </c>
+      <c r="H228" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -8325,20 +8328,20 @@
       <c r="C229" t="s">
         <v>563</v>
       </c>
-      <c r="D229">
-        <v>0</v>
-      </c>
-      <c r="E229">
-        <v>0</v>
-      </c>
-      <c r="F229">
-        <v>0</v>
-      </c>
-      <c r="G229">
-        <v>0</v>
-      </c>
-      <c r="H229">
-        <v>0</v>
+      <c r="D229" t="s">
+        <v>671</v>
+      </c>
+      <c r="E229" t="s">
+        <v>671</v>
+      </c>
+      <c r="F229" t="s">
+        <v>671</v>
+      </c>
+      <c r="G229" t="s">
+        <v>671</v>
+      </c>
+      <c r="H229" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -8351,20 +8354,20 @@
       <c r="C230" t="s">
         <v>564</v>
       </c>
-      <c r="D230">
-        <v>0</v>
-      </c>
-      <c r="E230">
-        <v>0</v>
-      </c>
-      <c r="F230">
-        <v>0</v>
-      </c>
-      <c r="G230">
-        <v>0</v>
-      </c>
-      <c r="H230">
-        <v>0</v>
+      <c r="D230" t="s">
+        <v>671</v>
+      </c>
+      <c r="E230" t="s">
+        <v>671</v>
+      </c>
+      <c r="F230" t="s">
+        <v>671</v>
+      </c>
+      <c r="G230" t="s">
+        <v>671</v>
+      </c>
+      <c r="H230" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -8377,20 +8380,20 @@
       <c r="C231" t="s">
         <v>565</v>
       </c>
-      <c r="D231">
-        <v>0</v>
-      </c>
-      <c r="E231">
-        <v>0</v>
-      </c>
-      <c r="F231">
-        <v>0</v>
-      </c>
-      <c r="G231">
-        <v>0</v>
-      </c>
-      <c r="H231">
-        <v>0</v>
+      <c r="D231" t="s">
+        <v>671</v>
+      </c>
+      <c r="E231" t="s">
+        <v>671</v>
+      </c>
+      <c r="F231" t="s">
+        <v>671</v>
+      </c>
+      <c r="G231" t="s">
+        <v>671</v>
+      </c>
+      <c r="H231" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -8403,20 +8406,20 @@
       <c r="C232" t="s">
         <v>566</v>
       </c>
-      <c r="D232">
-        <v>0</v>
-      </c>
-      <c r="E232">
-        <v>0</v>
-      </c>
-      <c r="F232">
-        <v>0</v>
-      </c>
-      <c r="G232">
-        <v>0</v>
-      </c>
-      <c r="H232">
-        <v>0</v>
+      <c r="D232" t="s">
+        <v>671</v>
+      </c>
+      <c r="E232" t="s">
+        <v>671</v>
+      </c>
+      <c r="F232" t="s">
+        <v>671</v>
+      </c>
+      <c r="G232" t="s">
+        <v>671</v>
+      </c>
+      <c r="H232" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -8429,20 +8432,20 @@
       <c r="C233" t="s">
         <v>567</v>
       </c>
-      <c r="D233">
-        <v>0</v>
-      </c>
-      <c r="E233">
-        <v>0</v>
-      </c>
-      <c r="F233">
-        <v>0</v>
-      </c>
-      <c r="G233">
-        <v>0</v>
-      </c>
-      <c r="H233">
-        <v>0</v>
+      <c r="D233" t="s">
+        <v>671</v>
+      </c>
+      <c r="E233" t="s">
+        <v>671</v>
+      </c>
+      <c r="F233" t="s">
+        <v>671</v>
+      </c>
+      <c r="G233" t="s">
+        <v>671</v>
+      </c>
+      <c r="H233" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -8455,20 +8458,20 @@
       <c r="C234" t="s">
         <v>568</v>
       </c>
-      <c r="D234">
-        <v>0</v>
-      </c>
-      <c r="E234">
-        <v>0</v>
-      </c>
-      <c r="F234">
-        <v>0</v>
-      </c>
-      <c r="G234">
-        <v>0</v>
-      </c>
-      <c r="H234">
-        <v>0</v>
+      <c r="D234" t="s">
+        <v>671</v>
+      </c>
+      <c r="E234" t="s">
+        <v>671</v>
+      </c>
+      <c r="F234" t="s">
+        <v>671</v>
+      </c>
+      <c r="G234" t="s">
+        <v>671</v>
+      </c>
+      <c r="H234" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -8481,20 +8484,20 @@
       <c r="C235" t="s">
         <v>569</v>
       </c>
-      <c r="D235">
-        <v>0</v>
-      </c>
-      <c r="E235">
-        <v>0</v>
-      </c>
-      <c r="F235">
-        <v>0</v>
-      </c>
-      <c r="G235">
-        <v>0</v>
-      </c>
-      <c r="H235">
-        <v>0</v>
+      <c r="D235" t="s">
+        <v>671</v>
+      </c>
+      <c r="E235" t="s">
+        <v>671</v>
+      </c>
+      <c r="F235" t="s">
+        <v>671</v>
+      </c>
+      <c r="G235" t="s">
+        <v>671</v>
+      </c>
+      <c r="H235" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -8507,20 +8510,20 @@
       <c r="C236" t="s">
         <v>570</v>
       </c>
-      <c r="D236">
-        <v>0</v>
-      </c>
-      <c r="E236">
-        <v>0</v>
-      </c>
-      <c r="F236">
-        <v>0</v>
-      </c>
-      <c r="G236">
-        <v>0</v>
-      </c>
-      <c r="H236">
-        <v>0</v>
+      <c r="D236" t="s">
+        <v>671</v>
+      </c>
+      <c r="E236" t="s">
+        <v>671</v>
+      </c>
+      <c r="F236" t="s">
+        <v>671</v>
+      </c>
+      <c r="G236" t="s">
+        <v>671</v>
+      </c>
+      <c r="H236" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -8533,20 +8536,20 @@
       <c r="C237" t="s">
         <v>571</v>
       </c>
-      <c r="D237">
-        <v>0</v>
-      </c>
-      <c r="E237">
-        <v>0</v>
-      </c>
-      <c r="F237">
-        <v>0</v>
-      </c>
-      <c r="G237">
-        <v>0</v>
-      </c>
-      <c r="H237">
-        <v>0</v>
+      <c r="D237" t="s">
+        <v>671</v>
+      </c>
+      <c r="E237" t="s">
+        <v>671</v>
+      </c>
+      <c r="F237" t="s">
+        <v>671</v>
+      </c>
+      <c r="G237" t="s">
+        <v>671</v>
+      </c>
+      <c r="H237" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -8559,20 +8562,20 @@
       <c r="C238" t="s">
         <v>572</v>
       </c>
-      <c r="D238">
-        <v>0</v>
-      </c>
-      <c r="E238">
-        <v>0</v>
-      </c>
-      <c r="F238">
-        <v>0</v>
-      </c>
-      <c r="G238">
-        <v>0</v>
-      </c>
-      <c r="H238">
-        <v>0</v>
+      <c r="D238" t="s">
+        <v>671</v>
+      </c>
+      <c r="E238" t="s">
+        <v>671</v>
+      </c>
+      <c r="F238" t="s">
+        <v>671</v>
+      </c>
+      <c r="G238" t="s">
+        <v>671</v>
+      </c>
+      <c r="H238" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -8585,20 +8588,20 @@
       <c r="C239" t="s">
         <v>573</v>
       </c>
-      <c r="D239">
-        <v>0</v>
-      </c>
-      <c r="E239">
-        <v>0</v>
-      </c>
-      <c r="F239">
-        <v>0</v>
-      </c>
-      <c r="G239">
-        <v>0</v>
-      </c>
-      <c r="H239">
-        <v>0</v>
+      <c r="D239" t="s">
+        <v>671</v>
+      </c>
+      <c r="E239" t="s">
+        <v>671</v>
+      </c>
+      <c r="F239" t="s">
+        <v>671</v>
+      </c>
+      <c r="G239" t="s">
+        <v>671</v>
+      </c>
+      <c r="H239" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -8611,20 +8614,20 @@
       <c r="C240" t="s">
         <v>574</v>
       </c>
-      <c r="D240">
-        <v>0</v>
-      </c>
-      <c r="E240">
-        <v>0</v>
-      </c>
-      <c r="F240">
-        <v>0</v>
-      </c>
-      <c r="G240">
-        <v>0</v>
-      </c>
-      <c r="H240">
-        <v>0</v>
+      <c r="D240" t="s">
+        <v>671</v>
+      </c>
+      <c r="E240" t="s">
+        <v>671</v>
+      </c>
+      <c r="F240" t="s">
+        <v>671</v>
+      </c>
+      <c r="G240" t="s">
+        <v>671</v>
+      </c>
+      <c r="H240" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8637,20 +8640,20 @@
       <c r="C241" t="s">
         <v>575</v>
       </c>
-      <c r="D241">
-        <v>0</v>
-      </c>
-      <c r="E241">
-        <v>0</v>
-      </c>
-      <c r="F241">
-        <v>0</v>
-      </c>
-      <c r="G241">
-        <v>0</v>
-      </c>
-      <c r="H241">
-        <v>0</v>
+      <c r="D241" t="s">
+        <v>671</v>
+      </c>
+      <c r="E241" t="s">
+        <v>671</v>
+      </c>
+      <c r="F241" t="s">
+        <v>671</v>
+      </c>
+      <c r="G241" t="s">
+        <v>671</v>
+      </c>
+      <c r="H241" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8663,20 +8666,20 @@
       <c r="C242" t="s">
         <v>576</v>
       </c>
-      <c r="D242">
-        <v>0</v>
-      </c>
-      <c r="E242">
-        <v>0</v>
-      </c>
-      <c r="F242">
-        <v>0</v>
-      </c>
-      <c r="G242">
-        <v>0</v>
-      </c>
-      <c r="H242">
-        <v>0</v>
+      <c r="D242" t="s">
+        <v>671</v>
+      </c>
+      <c r="E242" t="s">
+        <v>671</v>
+      </c>
+      <c r="F242" t="s">
+        <v>671</v>
+      </c>
+      <c r="G242" t="s">
+        <v>671</v>
+      </c>
+      <c r="H242" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8689,20 +8692,20 @@
       <c r="C243" t="s">
         <v>577</v>
       </c>
-      <c r="D243">
-        <v>0</v>
-      </c>
-      <c r="E243">
-        <v>0</v>
-      </c>
-      <c r="F243">
-        <v>0</v>
-      </c>
-      <c r="G243">
-        <v>0</v>
-      </c>
-      <c r="H243">
-        <v>0</v>
+      <c r="D243" t="s">
+        <v>671</v>
+      </c>
+      <c r="E243" t="s">
+        <v>671</v>
+      </c>
+      <c r="F243" t="s">
+        <v>671</v>
+      </c>
+      <c r="G243" t="s">
+        <v>671</v>
+      </c>
+      <c r="H243" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8715,20 +8718,20 @@
       <c r="C244" t="s">
         <v>578</v>
       </c>
-      <c r="D244">
-        <v>0</v>
-      </c>
-      <c r="E244">
-        <v>0</v>
-      </c>
-      <c r="F244">
-        <v>0</v>
-      </c>
-      <c r="G244">
-        <v>0</v>
-      </c>
-      <c r="H244">
-        <v>0</v>
+      <c r="D244" t="s">
+        <v>671</v>
+      </c>
+      <c r="E244" t="s">
+        <v>671</v>
+      </c>
+      <c r="F244" t="s">
+        <v>671</v>
+      </c>
+      <c r="G244" t="s">
+        <v>671</v>
+      </c>
+      <c r="H244" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8741,20 +8744,20 @@
       <c r="C245" t="s">
         <v>579</v>
       </c>
-      <c r="D245">
-        <v>0</v>
-      </c>
-      <c r="E245">
-        <v>0</v>
-      </c>
-      <c r="F245">
-        <v>0</v>
-      </c>
-      <c r="G245">
-        <v>0</v>
-      </c>
-      <c r="H245">
-        <v>0</v>
+      <c r="D245" t="s">
+        <v>671</v>
+      </c>
+      <c r="E245" t="s">
+        <v>671</v>
+      </c>
+      <c r="F245" t="s">
+        <v>671</v>
+      </c>
+      <c r="G245" t="s">
+        <v>671</v>
+      </c>
+      <c r="H245" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8767,20 +8770,20 @@
       <c r="C246" t="s">
         <v>580</v>
       </c>
-      <c r="D246">
-        <v>0</v>
-      </c>
-      <c r="E246">
-        <v>0</v>
-      </c>
-      <c r="F246">
-        <v>0</v>
-      </c>
-      <c r="G246">
-        <v>0</v>
-      </c>
-      <c r="H246">
-        <v>0</v>
+      <c r="D246" t="s">
+        <v>671</v>
+      </c>
+      <c r="E246" t="s">
+        <v>671</v>
+      </c>
+      <c r="F246" t="s">
+        <v>671</v>
+      </c>
+      <c r="G246" t="s">
+        <v>671</v>
+      </c>
+      <c r="H246" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8793,20 +8796,20 @@
       <c r="C247" t="s">
         <v>581</v>
       </c>
-      <c r="D247">
-        <v>0</v>
-      </c>
-      <c r="E247">
-        <v>0</v>
-      </c>
-      <c r="F247">
-        <v>0</v>
-      </c>
-      <c r="G247">
-        <v>0</v>
-      </c>
-      <c r="H247">
-        <v>0</v>
+      <c r="D247" t="s">
+        <v>671</v>
+      </c>
+      <c r="E247" t="s">
+        <v>671</v>
+      </c>
+      <c r="F247" t="s">
+        <v>671</v>
+      </c>
+      <c r="G247" t="s">
+        <v>671</v>
+      </c>
+      <c r="H247" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8819,20 +8822,20 @@
       <c r="C248" t="s">
         <v>582</v>
       </c>
-      <c r="D248">
-        <v>0</v>
-      </c>
-      <c r="E248">
-        <v>0</v>
-      </c>
-      <c r="F248">
-        <v>0</v>
-      </c>
-      <c r="G248">
-        <v>0</v>
-      </c>
-      <c r="H248">
-        <v>0</v>
+      <c r="D248" t="s">
+        <v>671</v>
+      </c>
+      <c r="E248" t="s">
+        <v>671</v>
+      </c>
+      <c r="F248" t="s">
+        <v>671</v>
+      </c>
+      <c r="G248" t="s">
+        <v>671</v>
+      </c>
+      <c r="H248" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8845,20 +8848,20 @@
       <c r="C249" t="s">
         <v>583</v>
       </c>
-      <c r="D249">
-        <v>0</v>
-      </c>
-      <c r="E249">
-        <v>0</v>
-      </c>
-      <c r="F249">
-        <v>0</v>
-      </c>
-      <c r="G249">
-        <v>0</v>
-      </c>
-      <c r="H249">
-        <v>0</v>
+      <c r="D249" t="s">
+        <v>671</v>
+      </c>
+      <c r="E249" t="s">
+        <v>671</v>
+      </c>
+      <c r="F249" t="s">
+        <v>671</v>
+      </c>
+      <c r="G249" t="s">
+        <v>671</v>
+      </c>
+      <c r="H249" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8871,20 +8874,20 @@
       <c r="C250" t="s">
         <v>584</v>
       </c>
-      <c r="D250">
-        <v>0</v>
-      </c>
-      <c r="E250">
-        <v>0</v>
-      </c>
-      <c r="F250">
-        <v>0</v>
-      </c>
-      <c r="G250">
-        <v>0</v>
-      </c>
-      <c r="H250">
-        <v>0</v>
+      <c r="D250" t="s">
+        <v>671</v>
+      </c>
+      <c r="E250" t="s">
+        <v>671</v>
+      </c>
+      <c r="F250" t="s">
+        <v>671</v>
+      </c>
+      <c r="G250" t="s">
+        <v>671</v>
+      </c>
+      <c r="H250" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8897,20 +8900,20 @@
       <c r="C251" t="s">
         <v>585</v>
       </c>
-      <c r="D251">
-        <v>0</v>
-      </c>
-      <c r="E251">
-        <v>0</v>
-      </c>
-      <c r="F251">
-        <v>0</v>
-      </c>
-      <c r="G251">
-        <v>0</v>
-      </c>
-      <c r="H251">
-        <v>0</v>
+      <c r="D251" t="s">
+        <v>671</v>
+      </c>
+      <c r="E251" t="s">
+        <v>671</v>
+      </c>
+      <c r="F251" t="s">
+        <v>671</v>
+      </c>
+      <c r="G251" t="s">
+        <v>671</v>
+      </c>
+      <c r="H251" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8923,20 +8926,20 @@
       <c r="C252" t="s">
         <v>586</v>
       </c>
-      <c r="D252">
-        <v>0</v>
-      </c>
-      <c r="E252">
-        <v>0</v>
-      </c>
-      <c r="F252">
-        <v>0</v>
-      </c>
-      <c r="G252">
-        <v>0</v>
-      </c>
-      <c r="H252">
-        <v>0</v>
+      <c r="D252" t="s">
+        <v>671</v>
+      </c>
+      <c r="E252" t="s">
+        <v>671</v>
+      </c>
+      <c r="F252" t="s">
+        <v>671</v>
+      </c>
+      <c r="G252" t="s">
+        <v>671</v>
+      </c>
+      <c r="H252" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8949,20 +8952,20 @@
       <c r="C253" t="s">
         <v>587</v>
       </c>
-      <c r="D253">
-        <v>0</v>
-      </c>
-      <c r="E253">
-        <v>0</v>
-      </c>
-      <c r="F253">
-        <v>0</v>
-      </c>
-      <c r="G253">
-        <v>0</v>
-      </c>
-      <c r="H253">
-        <v>0</v>
+      <c r="D253" t="s">
+        <v>671</v>
+      </c>
+      <c r="E253" t="s">
+        <v>671</v>
+      </c>
+      <c r="F253" t="s">
+        <v>671</v>
+      </c>
+      <c r="G253" t="s">
+        <v>671</v>
+      </c>
+      <c r="H253" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8975,20 +8978,20 @@
       <c r="C254" t="s">
         <v>588</v>
       </c>
-      <c r="D254">
-        <v>0</v>
-      </c>
-      <c r="E254">
-        <v>0</v>
-      </c>
-      <c r="F254">
-        <v>0</v>
-      </c>
-      <c r="G254">
-        <v>0</v>
-      </c>
-      <c r="H254">
-        <v>0</v>
+      <c r="D254" t="s">
+        <v>671</v>
+      </c>
+      <c r="E254" t="s">
+        <v>671</v>
+      </c>
+      <c r="F254" t="s">
+        <v>671</v>
+      </c>
+      <c r="G254" t="s">
+        <v>671</v>
+      </c>
+      <c r="H254" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -9001,20 +9004,20 @@
       <c r="C255" t="s">
         <v>589</v>
       </c>
-      <c r="D255">
-        <v>0</v>
-      </c>
-      <c r="E255">
-        <v>0</v>
-      </c>
-      <c r="F255">
-        <v>0</v>
-      </c>
-      <c r="G255">
-        <v>0</v>
-      </c>
-      <c r="H255">
-        <v>0</v>
+      <c r="D255" t="s">
+        <v>671</v>
+      </c>
+      <c r="E255" t="s">
+        <v>671</v>
+      </c>
+      <c r="F255" t="s">
+        <v>671</v>
+      </c>
+      <c r="G255" t="s">
+        <v>671</v>
+      </c>
+      <c r="H255" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -9027,20 +9030,20 @@
       <c r="C256" t="s">
         <v>590</v>
       </c>
-      <c r="D256">
-        <v>0</v>
-      </c>
-      <c r="E256">
-        <v>0</v>
-      </c>
-      <c r="F256">
-        <v>0</v>
-      </c>
-      <c r="G256">
-        <v>0</v>
-      </c>
-      <c r="H256">
-        <v>0</v>
+      <c r="D256" t="s">
+        <v>671</v>
+      </c>
+      <c r="E256" t="s">
+        <v>671</v>
+      </c>
+      <c r="F256" t="s">
+        <v>671</v>
+      </c>
+      <c r="G256" t="s">
+        <v>671</v>
+      </c>
+      <c r="H256" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -9053,20 +9056,20 @@
       <c r="C257" t="s">
         <v>591</v>
       </c>
-      <c r="D257">
-        <v>0</v>
-      </c>
-      <c r="E257">
-        <v>0</v>
-      </c>
-      <c r="F257">
-        <v>0</v>
-      </c>
-      <c r="G257">
-        <v>0</v>
-      </c>
-      <c r="H257">
-        <v>0</v>
+      <c r="D257" t="s">
+        <v>671</v>
+      </c>
+      <c r="E257" t="s">
+        <v>671</v>
+      </c>
+      <c r="F257" t="s">
+        <v>671</v>
+      </c>
+      <c r="G257" t="s">
+        <v>671</v>
+      </c>
+      <c r="H257" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -9079,20 +9082,20 @@
       <c r="C258" t="s">
         <v>592</v>
       </c>
-      <c r="D258">
-        <v>0</v>
-      </c>
-      <c r="E258">
-        <v>0</v>
-      </c>
-      <c r="F258">
-        <v>0</v>
-      </c>
-      <c r="G258">
-        <v>0</v>
-      </c>
-      <c r="H258">
-        <v>0</v>
+      <c r="D258" t="s">
+        <v>671</v>
+      </c>
+      <c r="E258" t="s">
+        <v>671</v>
+      </c>
+      <c r="F258" t="s">
+        <v>671</v>
+      </c>
+      <c r="G258" t="s">
+        <v>671</v>
+      </c>
+      <c r="H258" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -9105,20 +9108,20 @@
       <c r="C259" t="s">
         <v>593</v>
       </c>
-      <c r="D259">
-        <v>0</v>
-      </c>
-      <c r="E259">
-        <v>0</v>
-      </c>
-      <c r="F259">
-        <v>0</v>
-      </c>
-      <c r="G259">
-        <v>0</v>
-      </c>
-      <c r="H259">
-        <v>0</v>
+      <c r="D259" t="s">
+        <v>671</v>
+      </c>
+      <c r="E259" t="s">
+        <v>671</v>
+      </c>
+      <c r="F259" t="s">
+        <v>671</v>
+      </c>
+      <c r="G259" t="s">
+        <v>671</v>
+      </c>
+      <c r="H259" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -9131,20 +9134,20 @@
       <c r="C260" t="s">
         <v>594</v>
       </c>
-      <c r="D260">
-        <v>0</v>
-      </c>
-      <c r="E260">
-        <v>0</v>
-      </c>
-      <c r="F260">
-        <v>0</v>
-      </c>
-      <c r="G260">
-        <v>0</v>
-      </c>
-      <c r="H260">
-        <v>0</v>
+      <c r="D260" t="s">
+        <v>671</v>
+      </c>
+      <c r="E260" t="s">
+        <v>671</v>
+      </c>
+      <c r="F260" t="s">
+        <v>671</v>
+      </c>
+      <c r="G260" t="s">
+        <v>671</v>
+      </c>
+      <c r="H260" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -9157,20 +9160,20 @@
       <c r="C261" t="s">
         <v>595</v>
       </c>
-      <c r="D261">
-        <v>0</v>
-      </c>
-      <c r="E261">
-        <v>0</v>
-      </c>
-      <c r="F261">
-        <v>0</v>
-      </c>
-      <c r="G261">
-        <v>0</v>
-      </c>
-      <c r="H261">
-        <v>0</v>
+      <c r="D261" t="s">
+        <v>671</v>
+      </c>
+      <c r="E261" t="s">
+        <v>671</v>
+      </c>
+      <c r="F261" t="s">
+        <v>671</v>
+      </c>
+      <c r="G261" t="s">
+        <v>671</v>
+      </c>
+      <c r="H261" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -9183,20 +9186,20 @@
       <c r="C262" t="s">
         <v>596</v>
       </c>
-      <c r="D262">
-        <v>0</v>
-      </c>
-      <c r="E262">
-        <v>0</v>
-      </c>
-      <c r="F262">
-        <v>0</v>
-      </c>
-      <c r="G262">
-        <v>0</v>
-      </c>
-      <c r="H262">
-        <v>0</v>
+      <c r="D262" t="s">
+        <v>671</v>
+      </c>
+      <c r="E262" t="s">
+        <v>671</v>
+      </c>
+      <c r="F262" t="s">
+        <v>671</v>
+      </c>
+      <c r="G262" t="s">
+        <v>671</v>
+      </c>
+      <c r="H262" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -9209,20 +9212,20 @@
       <c r="C263" t="s">
         <v>597</v>
       </c>
-      <c r="D263">
-        <v>0</v>
-      </c>
-      <c r="E263">
-        <v>0</v>
-      </c>
-      <c r="F263">
-        <v>0</v>
-      </c>
-      <c r="G263">
-        <v>0</v>
-      </c>
-      <c r="H263">
-        <v>0</v>
+      <c r="D263" t="s">
+        <v>671</v>
+      </c>
+      <c r="E263" t="s">
+        <v>671</v>
+      </c>
+      <c r="F263" t="s">
+        <v>671</v>
+      </c>
+      <c r="G263" t="s">
+        <v>671</v>
+      </c>
+      <c r="H263" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="264" spans="1:8">
@@ -9235,20 +9238,20 @@
       <c r="C264" t="s">
         <v>598</v>
       </c>
-      <c r="D264">
-        <v>0</v>
-      </c>
-      <c r="E264">
-        <v>0</v>
-      </c>
-      <c r="F264">
-        <v>0</v>
-      </c>
-      <c r="G264">
-        <v>0</v>
-      </c>
-      <c r="H264">
-        <v>0</v>
+      <c r="D264" t="s">
+        <v>671</v>
+      </c>
+      <c r="E264" t="s">
+        <v>671</v>
+      </c>
+      <c r="F264" t="s">
+        <v>671</v>
+      </c>
+      <c r="G264" t="s">
+        <v>671</v>
+      </c>
+      <c r="H264" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="265" spans="1:8">
@@ -9261,20 +9264,20 @@
       <c r="C265" t="s">
         <v>598</v>
       </c>
-      <c r="D265">
-        <v>0</v>
-      </c>
-      <c r="E265">
-        <v>0</v>
-      </c>
-      <c r="F265">
-        <v>0</v>
-      </c>
-      <c r="G265">
-        <v>0</v>
-      </c>
-      <c r="H265">
-        <v>0</v>
+      <c r="D265" t="s">
+        <v>671</v>
+      </c>
+      <c r="E265" t="s">
+        <v>671</v>
+      </c>
+      <c r="F265" t="s">
+        <v>671</v>
+      </c>
+      <c r="G265" t="s">
+        <v>671</v>
+      </c>
+      <c r="H265" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="266" spans="1:8">
@@ -9287,20 +9290,20 @@
       <c r="C266" t="s">
         <v>599</v>
       </c>
-      <c r="D266">
-        <v>0</v>
-      </c>
-      <c r="E266">
-        <v>0</v>
-      </c>
-      <c r="F266">
-        <v>0</v>
-      </c>
-      <c r="G266">
-        <v>0</v>
-      </c>
-      <c r="H266">
-        <v>0</v>
+      <c r="D266" t="s">
+        <v>671</v>
+      </c>
+      <c r="E266" t="s">
+        <v>671</v>
+      </c>
+      <c r="F266" t="s">
+        <v>671</v>
+      </c>
+      <c r="G266" t="s">
+        <v>671</v>
+      </c>
+      <c r="H266" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="267" spans="1:8">
@@ -9313,20 +9316,20 @@
       <c r="C267" t="s">
         <v>600</v>
       </c>
-      <c r="D267">
-        <v>0</v>
-      </c>
-      <c r="E267">
-        <v>0</v>
-      </c>
-      <c r="F267">
-        <v>0</v>
-      </c>
-      <c r="G267">
-        <v>0</v>
-      </c>
-      <c r="H267">
-        <v>0</v>
+      <c r="D267" t="s">
+        <v>671</v>
+      </c>
+      <c r="E267" t="s">
+        <v>671</v>
+      </c>
+      <c r="F267" t="s">
+        <v>671</v>
+      </c>
+      <c r="G267" t="s">
+        <v>671</v>
+      </c>
+      <c r="H267" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="268" spans="1:8">
@@ -9339,20 +9342,20 @@
       <c r="C268" t="s">
         <v>601</v>
       </c>
-      <c r="D268">
-        <v>0</v>
-      </c>
-      <c r="E268">
-        <v>0</v>
-      </c>
-      <c r="F268">
-        <v>0</v>
-      </c>
-      <c r="G268">
-        <v>0</v>
-      </c>
-      <c r="H268">
-        <v>0</v>
+      <c r="D268" t="s">
+        <v>671</v>
+      </c>
+      <c r="E268" t="s">
+        <v>671</v>
+      </c>
+      <c r="F268" t="s">
+        <v>671</v>
+      </c>
+      <c r="G268" t="s">
+        <v>671</v>
+      </c>
+      <c r="H268" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="269" spans="1:8">
@@ -9365,20 +9368,20 @@
       <c r="C269" t="s">
         <v>602</v>
       </c>
-      <c r="D269">
-        <v>0</v>
-      </c>
-      <c r="E269">
-        <v>0</v>
-      </c>
-      <c r="F269">
-        <v>0</v>
-      </c>
-      <c r="G269">
-        <v>0</v>
-      </c>
-      <c r="H269">
-        <v>0</v>
+      <c r="D269" t="s">
+        <v>671</v>
+      </c>
+      <c r="E269" t="s">
+        <v>671</v>
+      </c>
+      <c r="F269" t="s">
+        <v>671</v>
+      </c>
+      <c r="G269" t="s">
+        <v>671</v>
+      </c>
+      <c r="H269" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="270" spans="1:8">
@@ -9391,20 +9394,20 @@
       <c r="C270" t="s">
         <v>603</v>
       </c>
-      <c r="D270">
-        <v>0</v>
-      </c>
-      <c r="E270">
-        <v>0</v>
-      </c>
-      <c r="F270">
-        <v>0</v>
-      </c>
-      <c r="G270">
-        <v>0</v>
-      </c>
-      <c r="H270">
-        <v>0</v>
+      <c r="D270" t="s">
+        <v>671</v>
+      </c>
+      <c r="E270" t="s">
+        <v>671</v>
+      </c>
+      <c r="F270" t="s">
+        <v>671</v>
+      </c>
+      <c r="G270" t="s">
+        <v>671</v>
+      </c>
+      <c r="H270" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="271" spans="1:8">
@@ -9417,20 +9420,20 @@
       <c r="C271" t="s">
         <v>604</v>
       </c>
-      <c r="D271">
-        <v>0</v>
-      </c>
-      <c r="E271">
-        <v>0</v>
-      </c>
-      <c r="F271">
-        <v>0</v>
-      </c>
-      <c r="G271">
-        <v>0</v>
-      </c>
-      <c r="H271">
-        <v>0</v>
+      <c r="D271" t="s">
+        <v>671</v>
+      </c>
+      <c r="E271" t="s">
+        <v>671</v>
+      </c>
+      <c r="F271" t="s">
+        <v>671</v>
+      </c>
+      <c r="G271" t="s">
+        <v>671</v>
+      </c>
+      <c r="H271" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="272" spans="1:8">
@@ -9443,20 +9446,20 @@
       <c r="C272" t="s">
         <v>605</v>
       </c>
-      <c r="D272">
-        <v>0</v>
-      </c>
-      <c r="E272">
-        <v>0</v>
-      </c>
-      <c r="F272">
-        <v>0</v>
-      </c>
-      <c r="G272">
-        <v>0</v>
-      </c>
-      <c r="H272">
-        <v>0</v>
+      <c r="D272" t="s">
+        <v>671</v>
+      </c>
+      <c r="E272" t="s">
+        <v>671</v>
+      </c>
+      <c r="F272" t="s">
+        <v>671</v>
+      </c>
+      <c r="G272" t="s">
+        <v>671</v>
+      </c>
+      <c r="H272" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="273" spans="1:8">
@@ -9469,20 +9472,20 @@
       <c r="C273" t="s">
         <v>606</v>
       </c>
-      <c r="D273">
-        <v>0</v>
-      </c>
-      <c r="E273">
-        <v>0</v>
-      </c>
-      <c r="F273">
-        <v>0</v>
-      </c>
-      <c r="G273">
-        <v>0</v>
-      </c>
-      <c r="H273">
-        <v>0</v>
+      <c r="D273" t="s">
+        <v>671</v>
+      </c>
+      <c r="E273" t="s">
+        <v>671</v>
+      </c>
+      <c r="F273" t="s">
+        <v>671</v>
+      </c>
+      <c r="G273" t="s">
+        <v>671</v>
+      </c>
+      <c r="H273" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="274" spans="1:8">
@@ -9495,20 +9498,20 @@
       <c r="C274" t="s">
         <v>607</v>
       </c>
-      <c r="D274">
-        <v>0</v>
-      </c>
-      <c r="E274">
-        <v>0</v>
-      </c>
-      <c r="F274">
-        <v>0</v>
-      </c>
-      <c r="G274">
-        <v>0</v>
-      </c>
-      <c r="H274">
-        <v>0</v>
+      <c r="D274" t="s">
+        <v>671</v>
+      </c>
+      <c r="E274" t="s">
+        <v>671</v>
+      </c>
+      <c r="F274" t="s">
+        <v>671</v>
+      </c>
+      <c r="G274" t="s">
+        <v>671</v>
+      </c>
+      <c r="H274" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="275" spans="1:8">
@@ -9521,20 +9524,20 @@
       <c r="C275" t="s">
         <v>608</v>
       </c>
-      <c r="D275">
-        <v>0</v>
-      </c>
-      <c r="E275">
-        <v>0</v>
-      </c>
-      <c r="F275">
-        <v>0</v>
-      </c>
-      <c r="G275">
-        <v>0</v>
-      </c>
-      <c r="H275">
-        <v>0</v>
+      <c r="D275" t="s">
+        <v>671</v>
+      </c>
+      <c r="E275" t="s">
+        <v>671</v>
+      </c>
+      <c r="F275" t="s">
+        <v>671</v>
+      </c>
+      <c r="G275" t="s">
+        <v>671</v>
+      </c>
+      <c r="H275" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="276" spans="1:8">
@@ -9547,20 +9550,20 @@
       <c r="C276" t="s">
         <v>609</v>
       </c>
-      <c r="D276">
-        <v>0</v>
-      </c>
-      <c r="E276">
-        <v>0</v>
-      </c>
-      <c r="F276">
-        <v>0</v>
-      </c>
-      <c r="G276">
-        <v>0</v>
-      </c>
-      <c r="H276">
-        <v>0</v>
+      <c r="D276" t="s">
+        <v>671</v>
+      </c>
+      <c r="E276" t="s">
+        <v>671</v>
+      </c>
+      <c r="F276" t="s">
+        <v>671</v>
+      </c>
+      <c r="G276" t="s">
+        <v>671</v>
+      </c>
+      <c r="H276" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="277" spans="1:8">
@@ -9573,20 +9576,20 @@
       <c r="C277" t="s">
         <v>610</v>
       </c>
-      <c r="D277">
-        <v>0</v>
-      </c>
-      <c r="E277">
-        <v>0</v>
-      </c>
-      <c r="F277">
-        <v>0</v>
-      </c>
-      <c r="G277">
-        <v>0</v>
-      </c>
-      <c r="H277">
-        <v>0</v>
+      <c r="D277" t="s">
+        <v>671</v>
+      </c>
+      <c r="E277" t="s">
+        <v>671</v>
+      </c>
+      <c r="F277" t="s">
+        <v>671</v>
+      </c>
+      <c r="G277" t="s">
+        <v>671</v>
+      </c>
+      <c r="H277" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="278" spans="1:8">
@@ -9599,20 +9602,20 @@
       <c r="C278" t="s">
         <v>611</v>
       </c>
-      <c r="D278">
-        <v>0</v>
-      </c>
-      <c r="E278">
-        <v>0</v>
-      </c>
-      <c r="F278">
-        <v>0</v>
-      </c>
-      <c r="G278">
-        <v>0</v>
-      </c>
-      <c r="H278">
-        <v>0</v>
+      <c r="D278" t="s">
+        <v>671</v>
+      </c>
+      <c r="E278" t="s">
+        <v>671</v>
+      </c>
+      <c r="F278" t="s">
+        <v>671</v>
+      </c>
+      <c r="G278" t="s">
+        <v>671</v>
+      </c>
+      <c r="H278" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="279" spans="1:8">
@@ -9625,20 +9628,20 @@
       <c r="C279" t="s">
         <v>612</v>
       </c>
-      <c r="D279">
-        <v>0</v>
-      </c>
-      <c r="E279">
-        <v>0</v>
-      </c>
-      <c r="F279">
-        <v>0</v>
-      </c>
-      <c r="G279">
-        <v>0</v>
-      </c>
-      <c r="H279">
-        <v>0</v>
+      <c r="D279" t="s">
+        <v>671</v>
+      </c>
+      <c r="E279" t="s">
+        <v>671</v>
+      </c>
+      <c r="F279" t="s">
+        <v>671</v>
+      </c>
+      <c r="G279" t="s">
+        <v>671</v>
+      </c>
+      <c r="H279" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="280" spans="1:8">
@@ -9651,20 +9654,20 @@
       <c r="C280" t="s">
         <v>613</v>
       </c>
-      <c r="D280">
-        <v>0</v>
-      </c>
-      <c r="E280">
-        <v>0</v>
-      </c>
-      <c r="F280">
-        <v>0</v>
-      </c>
-      <c r="G280">
-        <v>0</v>
-      </c>
-      <c r="H280">
-        <v>0</v>
+      <c r="D280" t="s">
+        <v>671</v>
+      </c>
+      <c r="E280" t="s">
+        <v>671</v>
+      </c>
+      <c r="F280" t="s">
+        <v>671</v>
+      </c>
+      <c r="G280" t="s">
+        <v>671</v>
+      </c>
+      <c r="H280" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="281" spans="1:8">
@@ -9677,20 +9680,20 @@
       <c r="C281" t="s">
         <v>614</v>
       </c>
-      <c r="D281">
-        <v>0</v>
-      </c>
-      <c r="E281">
-        <v>0</v>
-      </c>
-      <c r="F281">
-        <v>0</v>
-      </c>
-      <c r="G281">
-        <v>0</v>
-      </c>
-      <c r="H281">
-        <v>0</v>
+      <c r="D281" t="s">
+        <v>671</v>
+      </c>
+      <c r="E281" t="s">
+        <v>671</v>
+      </c>
+      <c r="F281" t="s">
+        <v>671</v>
+      </c>
+      <c r="G281" t="s">
+        <v>671</v>
+      </c>
+      <c r="H281" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="282" spans="1:8">
@@ -9703,20 +9706,20 @@
       <c r="C282" t="s">
         <v>605</v>
       </c>
-      <c r="D282">
-        <v>0</v>
-      </c>
-      <c r="E282">
-        <v>0</v>
-      </c>
-      <c r="F282">
-        <v>0</v>
-      </c>
-      <c r="G282">
-        <v>0</v>
-      </c>
-      <c r="H282">
-        <v>0</v>
+      <c r="D282" t="s">
+        <v>671</v>
+      </c>
+      <c r="E282" t="s">
+        <v>671</v>
+      </c>
+      <c r="F282" t="s">
+        <v>671</v>
+      </c>
+      <c r="G282" t="s">
+        <v>671</v>
+      </c>
+      <c r="H282" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="283" spans="1:8">
@@ -9729,20 +9732,20 @@
       <c r="C283" t="s">
         <v>615</v>
       </c>
-      <c r="D283">
-        <v>0</v>
-      </c>
-      <c r="E283">
-        <v>0</v>
-      </c>
-      <c r="F283">
-        <v>0</v>
-      </c>
-      <c r="G283">
-        <v>0</v>
-      </c>
-      <c r="H283">
-        <v>0</v>
+      <c r="D283" t="s">
+        <v>671</v>
+      </c>
+      <c r="E283" t="s">
+        <v>671</v>
+      </c>
+      <c r="F283" t="s">
+        <v>671</v>
+      </c>
+      <c r="G283" t="s">
+        <v>671</v>
+      </c>
+      <c r="H283" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="284" spans="1:8">
@@ -9755,20 +9758,20 @@
       <c r="C284" t="s">
         <v>616</v>
       </c>
-      <c r="D284">
-        <v>0</v>
-      </c>
-      <c r="E284">
-        <v>0</v>
-      </c>
-      <c r="F284">
-        <v>0</v>
-      </c>
-      <c r="G284">
-        <v>0</v>
-      </c>
-      <c r="H284">
-        <v>0</v>
+      <c r="D284" t="s">
+        <v>671</v>
+      </c>
+      <c r="E284" t="s">
+        <v>671</v>
+      </c>
+      <c r="F284" t="s">
+        <v>671</v>
+      </c>
+      <c r="G284" t="s">
+        <v>671</v>
+      </c>
+      <c r="H284" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="285" spans="1:8">
@@ -9781,20 +9784,20 @@
       <c r="C285" t="s">
         <v>617</v>
       </c>
-      <c r="D285">
-        <v>0</v>
-      </c>
-      <c r="E285">
-        <v>0</v>
-      </c>
-      <c r="F285">
-        <v>0</v>
-      </c>
-      <c r="G285">
-        <v>0</v>
-      </c>
-      <c r="H285">
-        <v>0</v>
+      <c r="D285" t="s">
+        <v>671</v>
+      </c>
+      <c r="E285" t="s">
+        <v>671</v>
+      </c>
+      <c r="F285" t="s">
+        <v>671</v>
+      </c>
+      <c r="G285" t="s">
+        <v>671</v>
+      </c>
+      <c r="H285" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="286" spans="1:8">
@@ -9807,20 +9810,20 @@
       <c r="C286" t="s">
         <v>618</v>
       </c>
-      <c r="D286">
-        <v>0</v>
-      </c>
-      <c r="E286">
-        <v>0</v>
-      </c>
-      <c r="F286">
-        <v>0</v>
-      </c>
-      <c r="G286">
-        <v>0</v>
-      </c>
-      <c r="H286">
-        <v>0</v>
+      <c r="D286" t="s">
+        <v>671</v>
+      </c>
+      <c r="E286" t="s">
+        <v>671</v>
+      </c>
+      <c r="F286" t="s">
+        <v>671</v>
+      </c>
+      <c r="G286" t="s">
+        <v>671</v>
+      </c>
+      <c r="H286" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="287" spans="1:8">
@@ -9833,20 +9836,20 @@
       <c r="C287" t="s">
         <v>619</v>
       </c>
-      <c r="D287">
-        <v>0</v>
-      </c>
-      <c r="E287">
-        <v>0</v>
-      </c>
-      <c r="F287">
-        <v>0</v>
-      </c>
-      <c r="G287">
-        <v>0</v>
-      </c>
-      <c r="H287">
-        <v>0</v>
+      <c r="D287" t="s">
+        <v>671</v>
+      </c>
+      <c r="E287" t="s">
+        <v>671</v>
+      </c>
+      <c r="F287" t="s">
+        <v>671</v>
+      </c>
+      <c r="G287" t="s">
+        <v>671</v>
+      </c>
+      <c r="H287" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="288" spans="1:8">
@@ -9859,20 +9862,20 @@
       <c r="C288" t="s">
         <v>610</v>
       </c>
-      <c r="D288">
-        <v>0</v>
-      </c>
-      <c r="E288">
-        <v>0</v>
-      </c>
-      <c r="F288">
-        <v>0</v>
-      </c>
-      <c r="G288">
-        <v>0</v>
-      </c>
-      <c r="H288">
-        <v>0</v>
+      <c r="D288" t="s">
+        <v>671</v>
+      </c>
+      <c r="E288" t="s">
+        <v>671</v>
+      </c>
+      <c r="F288" t="s">
+        <v>671</v>
+      </c>
+      <c r="G288" t="s">
+        <v>671</v>
+      </c>
+      <c r="H288" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="289" spans="1:8">
@@ -9885,20 +9888,20 @@
       <c r="C289" t="s">
         <v>620</v>
       </c>
-      <c r="D289">
-        <v>0</v>
-      </c>
-      <c r="E289">
-        <v>0</v>
-      </c>
-      <c r="F289">
-        <v>0</v>
-      </c>
-      <c r="G289">
-        <v>0</v>
-      </c>
-      <c r="H289">
-        <v>0</v>
+      <c r="D289" t="s">
+        <v>671</v>
+      </c>
+      <c r="E289" t="s">
+        <v>671</v>
+      </c>
+      <c r="F289" t="s">
+        <v>671</v>
+      </c>
+      <c r="G289" t="s">
+        <v>671</v>
+      </c>
+      <c r="H289" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="290" spans="1:8">
@@ -9911,20 +9914,20 @@
       <c r="C290" t="s">
         <v>621</v>
       </c>
-      <c r="D290">
-        <v>0</v>
-      </c>
-      <c r="E290">
-        <v>0</v>
-      </c>
-      <c r="F290">
-        <v>0</v>
-      </c>
-      <c r="G290">
-        <v>0</v>
-      </c>
-      <c r="H290">
-        <v>0</v>
+      <c r="D290" t="s">
+        <v>671</v>
+      </c>
+      <c r="E290" t="s">
+        <v>671</v>
+      </c>
+      <c r="F290" t="s">
+        <v>671</v>
+      </c>
+      <c r="G290" t="s">
+        <v>671</v>
+      </c>
+      <c r="H290" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="291" spans="1:8">
@@ -9937,20 +9940,20 @@
       <c r="C291" t="s">
         <v>622</v>
       </c>
-      <c r="D291">
-        <v>0</v>
-      </c>
-      <c r="E291">
-        <v>0</v>
-      </c>
-      <c r="F291">
-        <v>0</v>
-      </c>
-      <c r="G291">
-        <v>0</v>
-      </c>
-      <c r="H291">
-        <v>0</v>
+      <c r="D291" t="s">
+        <v>671</v>
+      </c>
+      <c r="E291" t="s">
+        <v>671</v>
+      </c>
+      <c r="F291" t="s">
+        <v>671</v>
+      </c>
+      <c r="G291" t="s">
+        <v>671</v>
+      </c>
+      <c r="H291" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="292" spans="1:8">
@@ -9963,20 +9966,20 @@
       <c r="C292" t="s">
         <v>623</v>
       </c>
-      <c r="D292">
-        <v>0</v>
-      </c>
-      <c r="E292">
-        <v>0</v>
-      </c>
-      <c r="F292">
-        <v>0</v>
-      </c>
-      <c r="G292">
-        <v>0</v>
-      </c>
-      <c r="H292">
-        <v>0</v>
+      <c r="D292" t="s">
+        <v>671</v>
+      </c>
+      <c r="E292" t="s">
+        <v>671</v>
+      </c>
+      <c r="F292" t="s">
+        <v>671</v>
+      </c>
+      <c r="G292" t="s">
+        <v>671</v>
+      </c>
+      <c r="H292" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="293" spans="1:8">
@@ -9989,20 +9992,20 @@
       <c r="C293" t="s">
         <v>624</v>
       </c>
-      <c r="D293">
-        <v>0</v>
-      </c>
-      <c r="E293">
-        <v>0</v>
-      </c>
-      <c r="F293">
-        <v>0</v>
-      </c>
-      <c r="G293">
-        <v>0</v>
-      </c>
-      <c r="H293">
-        <v>0</v>
+      <c r="D293" t="s">
+        <v>671</v>
+      </c>
+      <c r="E293" t="s">
+        <v>671</v>
+      </c>
+      <c r="F293" t="s">
+        <v>671</v>
+      </c>
+      <c r="G293" t="s">
+        <v>671</v>
+      </c>
+      <c r="H293" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="294" spans="1:8">
@@ -10015,20 +10018,20 @@
       <c r="C294" t="s">
         <v>625</v>
       </c>
-      <c r="D294">
-        <v>0</v>
-      </c>
-      <c r="E294">
-        <v>0</v>
-      </c>
-      <c r="F294">
-        <v>0</v>
-      </c>
-      <c r="G294">
-        <v>0</v>
-      </c>
-      <c r="H294">
-        <v>0</v>
+      <c r="D294" t="s">
+        <v>671</v>
+      </c>
+      <c r="E294" t="s">
+        <v>671</v>
+      </c>
+      <c r="F294" t="s">
+        <v>671</v>
+      </c>
+      <c r="G294" t="s">
+        <v>671</v>
+      </c>
+      <c r="H294" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="295" spans="1:8">
@@ -10041,20 +10044,20 @@
       <c r="C295" t="s">
         <v>626</v>
       </c>
-      <c r="D295">
-        <v>0</v>
-      </c>
-      <c r="E295">
-        <v>0</v>
-      </c>
-      <c r="F295">
-        <v>0</v>
-      </c>
-      <c r="G295">
-        <v>0</v>
-      </c>
-      <c r="H295">
-        <v>0</v>
+      <c r="D295" t="s">
+        <v>671</v>
+      </c>
+      <c r="E295" t="s">
+        <v>671</v>
+      </c>
+      <c r="F295" t="s">
+        <v>671</v>
+      </c>
+      <c r="G295" t="s">
+        <v>671</v>
+      </c>
+      <c r="H295" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="296" spans="1:8">
@@ -10067,20 +10070,20 @@
       <c r="C296" t="s">
         <v>627</v>
       </c>
-      <c r="D296">
-        <v>0</v>
-      </c>
-      <c r="E296">
-        <v>0</v>
-      </c>
-      <c r="F296">
-        <v>0</v>
-      </c>
-      <c r="G296">
-        <v>0</v>
-      </c>
-      <c r="H296">
-        <v>0</v>
+      <c r="D296" t="s">
+        <v>671</v>
+      </c>
+      <c r="E296" t="s">
+        <v>671</v>
+      </c>
+      <c r="F296" t="s">
+        <v>671</v>
+      </c>
+      <c r="G296" t="s">
+        <v>671</v>
+      </c>
+      <c r="H296" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="297" spans="1:8">
@@ -10093,20 +10096,20 @@
       <c r="C297" t="s">
         <v>628</v>
       </c>
-      <c r="D297">
-        <v>0</v>
-      </c>
-      <c r="E297">
-        <v>0</v>
-      </c>
-      <c r="F297">
-        <v>0</v>
-      </c>
-      <c r="G297">
-        <v>0</v>
-      </c>
-      <c r="H297">
-        <v>0</v>
+      <c r="D297" t="s">
+        <v>671</v>
+      </c>
+      <c r="E297" t="s">
+        <v>671</v>
+      </c>
+      <c r="F297" t="s">
+        <v>671</v>
+      </c>
+      <c r="G297" t="s">
+        <v>671</v>
+      </c>
+      <c r="H297" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="298" spans="1:8">
@@ -10119,20 +10122,20 @@
       <c r="C298" t="s">
         <v>629</v>
       </c>
-      <c r="D298">
-        <v>0</v>
-      </c>
-      <c r="E298">
-        <v>0</v>
-      </c>
-      <c r="F298">
-        <v>0</v>
-      </c>
-      <c r="G298">
-        <v>0</v>
-      </c>
-      <c r="H298">
-        <v>0</v>
+      <c r="D298" t="s">
+        <v>671</v>
+      </c>
+      <c r="E298" t="s">
+        <v>671</v>
+      </c>
+      <c r="F298" t="s">
+        <v>671</v>
+      </c>
+      <c r="G298" t="s">
+        <v>671</v>
+      </c>
+      <c r="H298" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="299" spans="1:8">
@@ -10145,20 +10148,20 @@
       <c r="C299" t="s">
         <v>630</v>
       </c>
-      <c r="D299">
-        <v>0</v>
-      </c>
-      <c r="E299">
-        <v>0</v>
-      </c>
-      <c r="F299">
-        <v>0</v>
-      </c>
-      <c r="G299">
-        <v>0</v>
-      </c>
-      <c r="H299">
-        <v>0</v>
+      <c r="D299" t="s">
+        <v>671</v>
+      </c>
+      <c r="E299" t="s">
+        <v>671</v>
+      </c>
+      <c r="F299" t="s">
+        <v>671</v>
+      </c>
+      <c r="G299" t="s">
+        <v>671</v>
+      </c>
+      <c r="H299" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="300" spans="1:8">
@@ -10171,20 +10174,20 @@
       <c r="C300" t="s">
         <v>631</v>
       </c>
-      <c r="D300">
-        <v>0</v>
-      </c>
-      <c r="E300">
-        <v>0</v>
-      </c>
-      <c r="F300">
-        <v>0</v>
-      </c>
-      <c r="G300">
-        <v>0</v>
-      </c>
-      <c r="H300">
-        <v>0</v>
+      <c r="D300" t="s">
+        <v>671</v>
+      </c>
+      <c r="E300" t="s">
+        <v>671</v>
+      </c>
+      <c r="F300" t="s">
+        <v>671</v>
+      </c>
+      <c r="G300" t="s">
+        <v>671</v>
+      </c>
+      <c r="H300" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="301" spans="1:8">
@@ -10197,20 +10200,20 @@
       <c r="C301" t="s">
         <v>632</v>
       </c>
-      <c r="D301">
-        <v>0</v>
-      </c>
-      <c r="E301">
-        <v>0</v>
-      </c>
-      <c r="F301">
-        <v>0</v>
-      </c>
-      <c r="G301">
-        <v>0</v>
-      </c>
-      <c r="H301">
-        <v>0</v>
+      <c r="D301" t="s">
+        <v>671</v>
+      </c>
+      <c r="E301" t="s">
+        <v>671</v>
+      </c>
+      <c r="F301" t="s">
+        <v>671</v>
+      </c>
+      <c r="G301" t="s">
+        <v>671</v>
+      </c>
+      <c r="H301" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="302" spans="1:8">
@@ -10223,20 +10226,20 @@
       <c r="C302" t="s">
         <v>633</v>
       </c>
-      <c r="D302">
-        <v>0</v>
-      </c>
-      <c r="E302">
-        <v>0</v>
-      </c>
-      <c r="F302">
-        <v>0</v>
-      </c>
-      <c r="G302">
-        <v>0</v>
-      </c>
-      <c r="H302">
-        <v>0</v>
+      <c r="D302" t="s">
+        <v>671</v>
+      </c>
+      <c r="E302" t="s">
+        <v>671</v>
+      </c>
+      <c r="F302" t="s">
+        <v>671</v>
+      </c>
+      <c r="G302" t="s">
+        <v>671</v>
+      </c>
+      <c r="H302" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="303" spans="1:8">
@@ -10249,20 +10252,20 @@
       <c r="C303" t="s">
         <v>634</v>
       </c>
-      <c r="D303">
-        <v>0</v>
-      </c>
-      <c r="E303">
-        <v>0</v>
-      </c>
-      <c r="F303">
-        <v>0</v>
-      </c>
-      <c r="G303">
-        <v>0</v>
-      </c>
-      <c r="H303">
-        <v>0</v>
+      <c r="D303" t="s">
+        <v>671</v>
+      </c>
+      <c r="E303" t="s">
+        <v>671</v>
+      </c>
+      <c r="F303" t="s">
+        <v>671</v>
+      </c>
+      <c r="G303" t="s">
+        <v>671</v>
+      </c>
+      <c r="H303" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="304" spans="1:8">
@@ -10275,20 +10278,20 @@
       <c r="C304" t="s">
         <v>635</v>
       </c>
-      <c r="D304">
-        <v>0</v>
-      </c>
-      <c r="E304">
-        <v>0</v>
-      </c>
-      <c r="F304">
-        <v>0</v>
-      </c>
-      <c r="G304">
-        <v>0</v>
-      </c>
-      <c r="H304">
-        <v>0</v>
+      <c r="D304" t="s">
+        <v>671</v>
+      </c>
+      <c r="E304" t="s">
+        <v>671</v>
+      </c>
+      <c r="F304" t="s">
+        <v>671</v>
+      </c>
+      <c r="G304" t="s">
+        <v>671</v>
+      </c>
+      <c r="H304" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="305" spans="1:8">
@@ -10301,20 +10304,20 @@
       <c r="C305" t="s">
         <v>636</v>
       </c>
-      <c r="D305">
-        <v>0</v>
-      </c>
-      <c r="E305">
-        <v>0</v>
-      </c>
-      <c r="F305">
-        <v>0</v>
-      </c>
-      <c r="G305">
-        <v>0</v>
-      </c>
-      <c r="H305">
-        <v>0</v>
+      <c r="D305" t="s">
+        <v>671</v>
+      </c>
+      <c r="E305" t="s">
+        <v>671</v>
+      </c>
+      <c r="F305" t="s">
+        <v>671</v>
+      </c>
+      <c r="G305" t="s">
+        <v>671</v>
+      </c>
+      <c r="H305" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="306" spans="1:8">
@@ -10327,20 +10330,20 @@
       <c r="C306" t="s">
         <v>637</v>
       </c>
-      <c r="D306">
-        <v>0</v>
-      </c>
-      <c r="E306">
-        <v>0</v>
-      </c>
-      <c r="F306">
-        <v>0</v>
-      </c>
-      <c r="G306">
-        <v>0</v>
-      </c>
-      <c r="H306">
-        <v>0</v>
+      <c r="D306" t="s">
+        <v>671</v>
+      </c>
+      <c r="E306" t="s">
+        <v>671</v>
+      </c>
+      <c r="F306" t="s">
+        <v>671</v>
+      </c>
+      <c r="G306" t="s">
+        <v>671</v>
+      </c>
+      <c r="H306" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="307" spans="1:8">
@@ -10353,20 +10356,20 @@
       <c r="C307" t="s">
         <v>638</v>
       </c>
-      <c r="D307">
-        <v>0</v>
-      </c>
-      <c r="E307">
-        <v>0</v>
-      </c>
-      <c r="F307">
-        <v>0</v>
-      </c>
-      <c r="G307">
-        <v>0</v>
-      </c>
-      <c r="H307">
-        <v>0</v>
+      <c r="D307" t="s">
+        <v>671</v>
+      </c>
+      <c r="E307" t="s">
+        <v>671</v>
+      </c>
+      <c r="F307" t="s">
+        <v>671</v>
+      </c>
+      <c r="G307" t="s">
+        <v>671</v>
+      </c>
+      <c r="H307" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="308" spans="1:8">
@@ -10379,20 +10382,20 @@
       <c r="C308" t="s">
         <v>639</v>
       </c>
-      <c r="D308">
-        <v>0</v>
-      </c>
-      <c r="E308">
-        <v>0</v>
-      </c>
-      <c r="F308">
-        <v>0</v>
-      </c>
-      <c r="G308">
-        <v>0</v>
-      </c>
-      <c r="H308">
-        <v>0</v>
+      <c r="D308" t="s">
+        <v>671</v>
+      </c>
+      <c r="E308" t="s">
+        <v>671</v>
+      </c>
+      <c r="F308" t="s">
+        <v>671</v>
+      </c>
+      <c r="G308" t="s">
+        <v>671</v>
+      </c>
+      <c r="H308" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="309" spans="1:8">
@@ -10405,20 +10408,20 @@
       <c r="C309" t="s">
         <v>640</v>
       </c>
-      <c r="D309">
-        <v>0</v>
-      </c>
-      <c r="E309">
-        <v>0</v>
-      </c>
-      <c r="F309">
-        <v>0</v>
-      </c>
-      <c r="G309">
-        <v>0</v>
-      </c>
-      <c r="H309">
-        <v>0</v>
+      <c r="D309" t="s">
+        <v>671</v>
+      </c>
+      <c r="E309" t="s">
+        <v>671</v>
+      </c>
+      <c r="F309" t="s">
+        <v>671</v>
+      </c>
+      <c r="G309" t="s">
+        <v>671</v>
+      </c>
+      <c r="H309" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -10431,20 +10434,20 @@
       <c r="C310" t="s">
         <v>641</v>
       </c>
-      <c r="D310">
-        <v>0</v>
-      </c>
-      <c r="E310">
-        <v>0</v>
-      </c>
-      <c r="F310">
-        <v>0</v>
-      </c>
-      <c r="G310">
-        <v>0</v>
-      </c>
-      <c r="H310">
-        <v>0</v>
+      <c r="D310" t="s">
+        <v>671</v>
+      </c>
+      <c r="E310" t="s">
+        <v>671</v>
+      </c>
+      <c r="F310" t="s">
+        <v>671</v>
+      </c>
+      <c r="G310" t="s">
+        <v>671</v>
+      </c>
+      <c r="H310" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="311" spans="1:8">
@@ -10457,20 +10460,20 @@
       <c r="C311" t="s">
         <v>642</v>
       </c>
-      <c r="D311">
-        <v>0</v>
-      </c>
-      <c r="E311">
-        <v>0</v>
-      </c>
-      <c r="F311">
-        <v>0</v>
-      </c>
-      <c r="G311">
-        <v>0</v>
-      </c>
-      <c r="H311">
-        <v>0</v>
+      <c r="D311" t="s">
+        <v>671</v>
+      </c>
+      <c r="E311" t="s">
+        <v>671</v>
+      </c>
+      <c r="F311" t="s">
+        <v>671</v>
+      </c>
+      <c r="G311" t="s">
+        <v>671</v>
+      </c>
+      <c r="H311" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="312" spans="1:8">
@@ -10483,20 +10486,20 @@
       <c r="C312" t="s">
         <v>643</v>
       </c>
-      <c r="D312">
-        <v>0</v>
-      </c>
-      <c r="E312">
-        <v>0</v>
-      </c>
-      <c r="F312">
-        <v>0</v>
-      </c>
-      <c r="G312">
-        <v>0</v>
-      </c>
-      <c r="H312">
-        <v>0</v>
+      <c r="D312" t="s">
+        <v>671</v>
+      </c>
+      <c r="E312" t="s">
+        <v>671</v>
+      </c>
+      <c r="F312" t="s">
+        <v>671</v>
+      </c>
+      <c r="G312" t="s">
+        <v>671</v>
+      </c>
+      <c r="H312" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="313" spans="1:8">
@@ -10509,20 +10512,20 @@
       <c r="C313" t="s">
         <v>644</v>
       </c>
-      <c r="D313">
-        <v>0</v>
-      </c>
-      <c r="E313">
-        <v>0</v>
-      </c>
-      <c r="F313">
-        <v>0</v>
-      </c>
-      <c r="G313">
-        <v>0</v>
-      </c>
-      <c r="H313">
-        <v>0</v>
+      <c r="D313" t="s">
+        <v>671</v>
+      </c>
+      <c r="E313" t="s">
+        <v>671</v>
+      </c>
+      <c r="F313" t="s">
+        <v>671</v>
+      </c>
+      <c r="G313" t="s">
+        <v>671</v>
+      </c>
+      <c r="H313" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="314" spans="1:8">
@@ -10535,20 +10538,20 @@
       <c r="C314" t="s">
         <v>645</v>
       </c>
-      <c r="D314">
-        <v>0</v>
-      </c>
-      <c r="E314">
-        <v>0</v>
-      </c>
-      <c r="F314">
-        <v>0</v>
-      </c>
-      <c r="G314">
-        <v>0</v>
-      </c>
-      <c r="H314">
-        <v>0</v>
+      <c r="D314" t="s">
+        <v>671</v>
+      </c>
+      <c r="E314" t="s">
+        <v>671</v>
+      </c>
+      <c r="F314" t="s">
+        <v>671</v>
+      </c>
+      <c r="G314" t="s">
+        <v>671</v>
+      </c>
+      <c r="H314" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="315" spans="1:8">
@@ -10561,20 +10564,20 @@
       <c r="C315" t="s">
         <v>646</v>
       </c>
-      <c r="D315">
-        <v>0</v>
-      </c>
-      <c r="E315">
-        <v>0</v>
-      </c>
-      <c r="F315">
-        <v>0</v>
-      </c>
-      <c r="G315">
-        <v>0</v>
-      </c>
-      <c r="H315">
-        <v>0</v>
+      <c r="D315" t="s">
+        <v>671</v>
+      </c>
+      <c r="E315" t="s">
+        <v>671</v>
+      </c>
+      <c r="F315" t="s">
+        <v>671</v>
+      </c>
+      <c r="G315" t="s">
+        <v>671</v>
+      </c>
+      <c r="H315" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="316" spans="1:8">
@@ -10587,20 +10590,20 @@
       <c r="C316" t="s">
         <v>647</v>
       </c>
-      <c r="D316">
-        <v>0</v>
-      </c>
-      <c r="E316">
-        <v>0</v>
-      </c>
-      <c r="F316">
-        <v>0</v>
-      </c>
-      <c r="G316">
-        <v>0</v>
-      </c>
-      <c r="H316">
-        <v>0</v>
+      <c r="D316" t="s">
+        <v>671</v>
+      </c>
+      <c r="E316" t="s">
+        <v>671</v>
+      </c>
+      <c r="F316" t="s">
+        <v>671</v>
+      </c>
+      <c r="G316" t="s">
+        <v>671</v>
+      </c>
+      <c r="H316" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="317" spans="1:8">
@@ -10613,20 +10616,20 @@
       <c r="C317" t="s">
         <v>648</v>
       </c>
-      <c r="D317">
-        <v>0</v>
-      </c>
-      <c r="E317">
-        <v>0</v>
-      </c>
-      <c r="F317">
-        <v>0</v>
-      </c>
-      <c r="G317">
-        <v>0</v>
-      </c>
-      <c r="H317">
-        <v>0</v>
+      <c r="D317" t="s">
+        <v>671</v>
+      </c>
+      <c r="E317" t="s">
+        <v>671</v>
+      </c>
+      <c r="F317" t="s">
+        <v>671</v>
+      </c>
+      <c r="G317" t="s">
+        <v>671</v>
+      </c>
+      <c r="H317" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="318" spans="1:8">
@@ -10639,20 +10642,20 @@
       <c r="C318" t="s">
         <v>649</v>
       </c>
-      <c r="D318">
-        <v>0</v>
-      </c>
-      <c r="E318">
-        <v>0</v>
-      </c>
-      <c r="F318">
-        <v>0</v>
-      </c>
-      <c r="G318">
-        <v>0</v>
-      </c>
-      <c r="H318">
-        <v>0</v>
+      <c r="D318" t="s">
+        <v>671</v>
+      </c>
+      <c r="E318" t="s">
+        <v>671</v>
+      </c>
+      <c r="F318" t="s">
+        <v>671</v>
+      </c>
+      <c r="G318" t="s">
+        <v>671</v>
+      </c>
+      <c r="H318" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="319" spans="1:8">
@@ -10665,20 +10668,20 @@
       <c r="C319" t="s">
         <v>650</v>
       </c>
-      <c r="D319">
-        <v>0</v>
-      </c>
-      <c r="E319">
-        <v>0</v>
-      </c>
-      <c r="F319">
-        <v>0</v>
-      </c>
-      <c r="G319">
-        <v>0</v>
-      </c>
-      <c r="H319">
-        <v>0</v>
+      <c r="D319" t="s">
+        <v>671</v>
+      </c>
+      <c r="E319" t="s">
+        <v>671</v>
+      </c>
+      <c r="F319" t="s">
+        <v>671</v>
+      </c>
+      <c r="G319" t="s">
+        <v>671</v>
+      </c>
+      <c r="H319" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="320" spans="1:8">
@@ -10691,20 +10694,20 @@
       <c r="C320" t="s">
         <v>651</v>
       </c>
-      <c r="D320">
-        <v>0</v>
-      </c>
-      <c r="E320">
-        <v>0</v>
-      </c>
-      <c r="F320">
-        <v>0</v>
-      </c>
-      <c r="G320">
-        <v>0</v>
-      </c>
-      <c r="H320">
-        <v>0</v>
+      <c r="D320" t="s">
+        <v>671</v>
+      </c>
+      <c r="E320" t="s">
+        <v>671</v>
+      </c>
+      <c r="F320" t="s">
+        <v>671</v>
+      </c>
+      <c r="G320" t="s">
+        <v>671</v>
+      </c>
+      <c r="H320" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="321" spans="1:8">
@@ -10717,20 +10720,20 @@
       <c r="C321" t="s">
         <v>652</v>
       </c>
-      <c r="D321">
-        <v>0</v>
-      </c>
-      <c r="E321">
-        <v>0</v>
-      </c>
-      <c r="F321">
-        <v>0</v>
-      </c>
-      <c r="G321">
-        <v>0</v>
-      </c>
-      <c r="H321">
-        <v>0</v>
+      <c r="D321" t="s">
+        <v>671</v>
+      </c>
+      <c r="E321" t="s">
+        <v>671</v>
+      </c>
+      <c r="F321" t="s">
+        <v>671</v>
+      </c>
+      <c r="G321" t="s">
+        <v>671</v>
+      </c>
+      <c r="H321" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="322" spans="1:8">
@@ -10743,20 +10746,20 @@
       <c r="C322" t="s">
         <v>653</v>
       </c>
-      <c r="D322">
-        <v>0</v>
-      </c>
-      <c r="E322">
-        <v>0</v>
-      </c>
-      <c r="F322">
-        <v>0</v>
-      </c>
-      <c r="G322">
-        <v>0</v>
-      </c>
-      <c r="H322">
-        <v>0</v>
+      <c r="D322" t="s">
+        <v>671</v>
+      </c>
+      <c r="E322" t="s">
+        <v>671</v>
+      </c>
+      <c r="F322" t="s">
+        <v>671</v>
+      </c>
+      <c r="G322" t="s">
+        <v>671</v>
+      </c>
+      <c r="H322" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="323" spans="1:8">
@@ -10769,20 +10772,20 @@
       <c r="C323" t="s">
         <v>654</v>
       </c>
-      <c r="D323">
-        <v>0</v>
-      </c>
-      <c r="E323">
-        <v>0</v>
-      </c>
-      <c r="F323">
-        <v>0</v>
-      </c>
-      <c r="G323">
-        <v>0</v>
-      </c>
-      <c r="H323">
-        <v>0</v>
+      <c r="D323" t="s">
+        <v>671</v>
+      </c>
+      <c r="E323" t="s">
+        <v>671</v>
+      </c>
+      <c r="F323" t="s">
+        <v>671</v>
+      </c>
+      <c r="G323" t="s">
+        <v>671</v>
+      </c>
+      <c r="H323" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="324" spans="1:8">
@@ -10795,20 +10798,20 @@
       <c r="C324" t="s">
         <v>655</v>
       </c>
-      <c r="D324">
-        <v>0</v>
-      </c>
-      <c r="E324">
-        <v>0</v>
-      </c>
-      <c r="F324">
-        <v>0</v>
-      </c>
-      <c r="G324">
-        <v>0</v>
-      </c>
-      <c r="H324">
-        <v>0</v>
+      <c r="D324" t="s">
+        <v>671</v>
+      </c>
+      <c r="E324" t="s">
+        <v>671</v>
+      </c>
+      <c r="F324" t="s">
+        <v>671</v>
+      </c>
+      <c r="G324" t="s">
+        <v>671</v>
+      </c>
+      <c r="H324" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="325" spans="1:8">
@@ -10821,20 +10824,20 @@
       <c r="C325" t="s">
         <v>656</v>
       </c>
-      <c r="D325">
-        <v>0</v>
-      </c>
-      <c r="E325">
-        <v>0</v>
-      </c>
-      <c r="F325">
-        <v>0</v>
-      </c>
-      <c r="G325">
-        <v>0</v>
-      </c>
-      <c r="H325">
-        <v>0</v>
+      <c r="D325" t="s">
+        <v>671</v>
+      </c>
+      <c r="E325" t="s">
+        <v>671</v>
+      </c>
+      <c r="F325" t="s">
+        <v>671</v>
+      </c>
+      <c r="G325" t="s">
+        <v>671</v>
+      </c>
+      <c r="H325" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="326" spans="1:8">
@@ -10847,20 +10850,20 @@
       <c r="C326" t="s">
         <v>657</v>
       </c>
-      <c r="D326">
-        <v>0</v>
-      </c>
-      <c r="E326">
-        <v>0</v>
-      </c>
-      <c r="F326">
-        <v>0</v>
-      </c>
-      <c r="G326">
-        <v>0</v>
-      </c>
-      <c r="H326">
-        <v>0</v>
+      <c r="D326" t="s">
+        <v>671</v>
+      </c>
+      <c r="E326" t="s">
+        <v>671</v>
+      </c>
+      <c r="F326" t="s">
+        <v>671</v>
+      </c>
+      <c r="G326" t="s">
+        <v>671</v>
+      </c>
+      <c r="H326" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="327" spans="1:8">
@@ -10873,20 +10876,20 @@
       <c r="C327" t="s">
         <v>658</v>
       </c>
-      <c r="D327">
-        <v>0</v>
-      </c>
-      <c r="E327">
-        <v>0</v>
-      </c>
-      <c r="F327">
-        <v>0</v>
-      </c>
-      <c r="G327">
-        <v>0</v>
-      </c>
-      <c r="H327">
-        <v>0</v>
+      <c r="D327" t="s">
+        <v>671</v>
+      </c>
+      <c r="E327" t="s">
+        <v>671</v>
+      </c>
+      <c r="F327" t="s">
+        <v>671</v>
+      </c>
+      <c r="G327" t="s">
+        <v>671</v>
+      </c>
+      <c r="H327" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="328" spans="1:8">
@@ -10899,20 +10902,20 @@
       <c r="C328" t="s">
         <v>659</v>
       </c>
-      <c r="D328">
-        <v>0</v>
-      </c>
-      <c r="E328">
-        <v>0</v>
-      </c>
-      <c r="F328">
-        <v>0</v>
-      </c>
-      <c r="G328">
-        <v>0</v>
-      </c>
-      <c r="H328">
-        <v>0</v>
+      <c r="D328" t="s">
+        <v>671</v>
+      </c>
+      <c r="E328" t="s">
+        <v>671</v>
+      </c>
+      <c r="F328" t="s">
+        <v>671</v>
+      </c>
+      <c r="G328" t="s">
+        <v>671</v>
+      </c>
+      <c r="H328" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="329" spans="1:8">
@@ -10925,20 +10928,20 @@
       <c r="C329" t="s">
         <v>660</v>
       </c>
-      <c r="D329">
-        <v>0</v>
-      </c>
-      <c r="E329">
-        <v>0</v>
-      </c>
-      <c r="F329">
-        <v>0</v>
-      </c>
-      <c r="G329">
-        <v>0</v>
-      </c>
-      <c r="H329">
-        <v>0</v>
+      <c r="D329" t="s">
+        <v>671</v>
+      </c>
+      <c r="E329" t="s">
+        <v>671</v>
+      </c>
+      <c r="F329" t="s">
+        <v>671</v>
+      </c>
+      <c r="G329" t="s">
+        <v>671</v>
+      </c>
+      <c r="H329" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="330" spans="1:8">
@@ -10951,20 +10954,20 @@
       <c r="C330" t="s">
         <v>661</v>
       </c>
-      <c r="D330">
-        <v>0</v>
-      </c>
-      <c r="E330">
-        <v>0</v>
-      </c>
-      <c r="F330">
-        <v>0</v>
-      </c>
-      <c r="G330">
-        <v>0</v>
-      </c>
-      <c r="H330">
-        <v>0</v>
+      <c r="D330" t="s">
+        <v>671</v>
+      </c>
+      <c r="E330" t="s">
+        <v>671</v>
+      </c>
+      <c r="F330" t="s">
+        <v>671</v>
+      </c>
+      <c r="G330" t="s">
+        <v>671</v>
+      </c>
+      <c r="H330" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="331" spans="1:8">
@@ -10977,20 +10980,20 @@
       <c r="C331" t="s">
         <v>662</v>
       </c>
-      <c r="D331">
-        <v>0</v>
-      </c>
-      <c r="E331">
-        <v>0</v>
-      </c>
-      <c r="F331">
-        <v>0</v>
-      </c>
-      <c r="G331">
-        <v>0</v>
-      </c>
-      <c r="H331">
-        <v>0</v>
+      <c r="D331" t="s">
+        <v>671</v>
+      </c>
+      <c r="E331" t="s">
+        <v>671</v>
+      </c>
+      <c r="F331" t="s">
+        <v>671</v>
+      </c>
+      <c r="G331" t="s">
+        <v>671</v>
+      </c>
+      <c r="H331" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="332" spans="1:8">
@@ -11003,20 +11006,20 @@
       <c r="C332" t="s">
         <v>663</v>
       </c>
-      <c r="D332">
-        <v>0</v>
-      </c>
-      <c r="E332">
-        <v>0</v>
-      </c>
-      <c r="F332">
-        <v>0</v>
-      </c>
-      <c r="G332">
-        <v>0</v>
-      </c>
-      <c r="H332">
-        <v>0</v>
+      <c r="D332" t="s">
+        <v>671</v>
+      </c>
+      <c r="E332" t="s">
+        <v>671</v>
+      </c>
+      <c r="F332" t="s">
+        <v>671</v>
+      </c>
+      <c r="G332" t="s">
+        <v>671</v>
+      </c>
+      <c r="H332" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="333" spans="1:8">
@@ -11029,20 +11032,20 @@
       <c r="C333" t="s">
         <v>445</v>
       </c>
-      <c r="D333">
-        <v>0</v>
-      </c>
-      <c r="E333">
-        <v>0</v>
-      </c>
-      <c r="F333">
-        <v>0</v>
-      </c>
-      <c r="G333">
-        <v>0</v>
-      </c>
-      <c r="H333">
-        <v>0</v>
+      <c r="D333" t="s">
+        <v>671</v>
+      </c>
+      <c r="E333" t="s">
+        <v>671</v>
+      </c>
+      <c r="F333" t="s">
+        <v>671</v>
+      </c>
+      <c r="G333" t="s">
+        <v>671</v>
+      </c>
+      <c r="H333" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="334" spans="1:8">
@@ -11055,20 +11058,20 @@
       <c r="C334" t="s">
         <v>664</v>
       </c>
-      <c r="D334">
-        <v>0</v>
-      </c>
-      <c r="E334">
-        <v>0</v>
-      </c>
-      <c r="F334">
-        <v>0</v>
-      </c>
-      <c r="G334">
-        <v>0</v>
-      </c>
-      <c r="H334">
-        <v>0</v>
+      <c r="D334" t="s">
+        <v>671</v>
+      </c>
+      <c r="E334" t="s">
+        <v>671</v>
+      </c>
+      <c r="F334" t="s">
+        <v>671</v>
+      </c>
+      <c r="G334" t="s">
+        <v>671</v>
+      </c>
+      <c r="H334" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="335" spans="1:8">
@@ -11081,20 +11084,20 @@
       <c r="C335" t="s">
         <v>665</v>
       </c>
-      <c r="D335">
-        <v>0</v>
-      </c>
-      <c r="E335">
-        <v>0</v>
-      </c>
-      <c r="F335">
-        <v>0</v>
-      </c>
-      <c r="G335">
-        <v>0</v>
-      </c>
-      <c r="H335">
-        <v>0</v>
+      <c r="D335" t="s">
+        <v>671</v>
+      </c>
+      <c r="E335" t="s">
+        <v>671</v>
+      </c>
+      <c r="F335" t="s">
+        <v>671</v>
+      </c>
+      <c r="G335" t="s">
+        <v>671</v>
+      </c>
+      <c r="H335" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="336" spans="1:8">
@@ -11107,20 +11110,20 @@
       <c r="C336" t="s">
         <v>666</v>
       </c>
-      <c r="D336">
-        <v>0</v>
-      </c>
-      <c r="E336">
-        <v>0</v>
-      </c>
-      <c r="F336">
-        <v>0</v>
-      </c>
-      <c r="G336">
-        <v>0</v>
-      </c>
-      <c r="H336">
-        <v>0</v>
+      <c r="D336" t="s">
+        <v>671</v>
+      </c>
+      <c r="E336" t="s">
+        <v>671</v>
+      </c>
+      <c r="F336" t="s">
+        <v>671</v>
+      </c>
+      <c r="G336" t="s">
+        <v>671</v>
+      </c>
+      <c r="H336" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="337" spans="1:8">
@@ -11133,20 +11136,20 @@
       <c r="C337" t="s">
         <v>667</v>
       </c>
-      <c r="D337">
-        <v>0</v>
-      </c>
-      <c r="E337">
-        <v>0</v>
-      </c>
-      <c r="F337">
-        <v>0</v>
-      </c>
-      <c r="G337">
-        <v>0</v>
-      </c>
-      <c r="H337">
-        <v>0</v>
+      <c r="D337" t="s">
+        <v>671</v>
+      </c>
+      <c r="E337" t="s">
+        <v>671</v>
+      </c>
+      <c r="F337" t="s">
+        <v>671</v>
+      </c>
+      <c r="G337" t="s">
+        <v>671</v>
+      </c>
+      <c r="H337" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="338" spans="1:8">
@@ -11159,20 +11162,20 @@
       <c r="C338" t="s">
         <v>668</v>
       </c>
-      <c r="D338">
-        <v>0</v>
-      </c>
-      <c r="E338">
-        <v>0</v>
-      </c>
-      <c r="F338">
-        <v>0</v>
-      </c>
-      <c r="G338">
-        <v>0</v>
-      </c>
-      <c r="H338">
-        <v>0</v>
+      <c r="D338" t="s">
+        <v>671</v>
+      </c>
+      <c r="E338" t="s">
+        <v>671</v>
+      </c>
+      <c r="F338" t="s">
+        <v>671</v>
+      </c>
+      <c r="G338" t="s">
+        <v>671</v>
+      </c>
+      <c r="H338" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="339" spans="1:8">
@@ -11185,20 +11188,20 @@
       <c r="C339" t="s">
         <v>669</v>
       </c>
-      <c r="D339">
-        <v>0</v>
-      </c>
-      <c r="E339">
-        <v>0</v>
-      </c>
-      <c r="F339">
-        <v>0</v>
-      </c>
-      <c r="G339">
-        <v>0</v>
-      </c>
-      <c r="H339">
-        <v>0</v>
+      <c r="D339" t="s">
+        <v>671</v>
+      </c>
+      <c r="E339" t="s">
+        <v>671</v>
+      </c>
+      <c r="F339" t="s">
+        <v>671</v>
+      </c>
+      <c r="G339" t="s">
+        <v>671</v>
+      </c>
+      <c r="H339" t="s">
+        <v>671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>